<commit_message>
COmmited on 28th april
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/LoginData.xlsx
+++ b/ocms/src/test/resources/TestData/LoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C86AF4-E86A-40E0-B398-E7448B127112}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D985C29-C65A-4783-8362-546112D7F07A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="45">
   <si>
     <t>Application URL</t>
   </si>
@@ -152,7 +152,10 @@
     <t>QATetherfi</t>
   </si>
   <si>
-    <t>Tetherfi@930</t>
+    <t>P@ssw0rd@123</t>
+  </si>
+  <si>
+    <t>meghna</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -539,10 +542,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>43</v>
@@ -808,10 +811,9 @@
     <hyperlink ref="C15" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="C16" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="C17" r:id="rId19" display="P@ssw0rd@123" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C2" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
agent aux report changes
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/LoginData.xlsx
+++ b/ocms/src/test/resources/TestData/LoginData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D69E3730-7F73-4F22-903F-ED0E4AA1E960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6B71CD-6AE0-4784-8963-CC64512E5A08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,11 @@
     <definedName name="UserType">Sheet1!$B$1:$B$3</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>Application URL</t>
   </si>
@@ -180,10 +179,7 @@
     <t>57ItuC6rG8(t!XlnPt*iC@-Ymwg)-DrX</t>
   </si>
   <si>
-    <t>testuser</t>
-  </si>
-  <si>
-    <t>Qwerty@135$</t>
+    <t>T3th3rfi987$</t>
   </si>
 </sst>
 </file>
@@ -533,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -549,7 +545,7 @@
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" customFormat="1">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -572,18 +568,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:7" customFormat="1">
+    <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>42</v>
@@ -592,7 +588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" customFormat="1">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>50</v>
       </c>
@@ -615,7 +611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" customFormat="1">
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -655,7 +651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" customFormat="1">
+    <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -675,7 +671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" customFormat="1">
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -695,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" customFormat="1">
+    <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -715,32 +711,32 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" customFormat="1">
+    <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" customFormat="1">
+    <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" customFormat="1">
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" customFormat="1">
+    <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" customFormat="1">
+    <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" customFormat="1">
+    <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -760,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" customFormat="1">
+    <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -777,7 +773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" customFormat="1">
+    <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
         <v>41</v>
       </c>
@@ -797,7 +793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" customFormat="1">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
         <v>41</v>
       </c>
@@ -817,17 +813,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7" customFormat="1">
+    <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:7" customFormat="1">
+    <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" customFormat="1">
+    <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
         <v>47</v>
       </c>
@@ -838,12 +834,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" customFormat="1">
+    <row r="21" spans="1:6">
       <c r="A21" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:7" customFormat="1"/>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:D17 D5 D14 D2" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -880,11 +875,9 @@
     <hyperlink ref="C20" r:id="rId24" display="P@ssw0rd@123" xr:uid="{A7D55041-56C9-412B-9DC6-1311F7751D64}"/>
     <hyperlink ref="A21" r:id="rId25" xr:uid="{A67C4A62-1E86-43BB-AA52-09BFC77A6E04}"/>
     <hyperlink ref="A3" r:id="rId26" xr:uid="{76877752-2E31-4FD9-A95E-B6ACC6AFB854}"/>
-    <hyperlink ref="A2" r:id="rId27" xr:uid="{34629AB9-D680-40ED-93AE-B6A5467CDE4B}"/>
-    <hyperlink ref="C2" r:id="rId28" xr:uid="{48D382D6-D0FF-4B38-BB19-049BD4FF554A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>